<commit_message>
Java+Spring [Shpping Mall] (Excel upload Finish)
</commit_message>
<xml_diff>
--- a/FashionShopNew/src/main/webapp/resources/excel/product_dump.xlsx
+++ b/FashionShopNew/src/main/webapp/resources/excel/product_dump.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\spring_workspace\FashionShop\src\main\webapp\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\spring_workspace\FashionShopNew\src\main\webapp\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C711E7B-F514-45E2-A993-8080EA752108}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F1CF03-B662-4EF4-8F9F-4FAAEBBC72BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="16896" windowHeight="8964" xr2:uid="{BFF4FE26-F889-412A-8A57-D98B99D80788}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BFF4FE26-F889-412A-8A57-D98B99D80788}"/>
   </bookViews>
   <sheets>
     <sheet name="product" sheetId="1" r:id="rId1"/>
@@ -200,7 +200,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>temp</t>
+    <t>temp.png</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -600,7 +600,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>

</xml_diff>